<commit_message>
Imp BTG pagamento de Salários por CNAB240
</commit_message>
<xml_diff>
--- a/etc/Manuais de Layouts/Tradutor CNAB - Pagamento.xlsx
+++ b/etc/Manuais de Layouts/Tradutor CNAB - Pagamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://btgpactual.sharepoint.com/sites/DreamTeamTeams/Documentos Compartilhados/General/Arquivos e Transmissões/Documentos/Kit CNAB/Febraban/Pagamento/Kit_CNAB_Pagamento/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\X\GH\rfw.finance\etc\Manuais de Layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{D2351CE2-FFAC-44C1-965B-B32F8E5E3D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55B23BC6-625B-4784-AC89-A210286D1F68}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0847AC3C-9CDC-47A7-B866-E0019C0D952D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{092A2AC9-8989-4EC8-B309-29E6D797AA17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28095" windowHeight="32400" xr2:uid="{092A2AC9-8989-4EC8-B309-29E6D797AA17}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -823,7 +823,7 @@
     <t xml:space="preserve">2080001300001J00020891976200000002000050011054458277103886850VECHI CONSULTORIA E PROJETOS L29062024000000000000200000000000000000000000000000000140620250000000000002000000000000000006d1711054458277     2106121711054458277109                </t>
   </si>
   <si>
-    <t xml:space="preserve">2080001300001A00001820800050 0000003742605 VIAS TESTE             LTDA   1337013495          06092024BRL000000000000000000000000000010                   000000000000000000000000                                                    0          </t>
+    <t xml:space="preserve">2080001300001A00000023703728 0000001385224 Rodrigo Gomes Macedo de Leitao0000000000000001437014032025BRL000000000000000000000000000100                    00000000000000000000000                                        06          0          </t>
   </si>
 </sst>
 </file>
@@ -3086,9 +3086,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3126,7 +3126,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3232,7 +3232,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3374,7 +3374,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3385,9 +3385,9 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A2:H39"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="F17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>018</v>
+        <v>000</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="F18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="F19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00050</v>
+        <v>03728</v>
       </c>
       <c r="G19" s="3"/>
     </row>
@@ -3679,7 +3679,7 @@
       </c>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>000000374260</v>
+        <v>000000138522</v>
       </c>
       <c r="G21" s="3"/>
     </row>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="F22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="F24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">VIAS TESTE             LTDA   </v>
+        <v>Rodrigo Gomes Macedo de Leitao</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="F25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">1337013495          </v>
+        <v>00000000000000014370</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -3774,7 +3774,7 @@
       </c>
       <c r="F26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>06092024</v>
+        <v>14032025</v>
       </c>
       <c r="G26" s="3"/>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="F29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>000000000000010</v>
+        <v>000000000000100</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -3850,7 +3850,7 @@
       </c>
       <c r="F30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                   0</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="F34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
+        <v>06</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -4047,7 +4047,7 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7:G7"/>
     </sheetView>
@@ -4387,7 +4387,7 @@
   <sheetPr codeName="Planilha3"/>
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
@@ -4841,9 +4841,9 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5333,8 +5333,8 @@
   <sheetPr codeName="Planilha5"/>
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -6158,7 +6158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78303EC6-3A45-487C-BF12-4E4BA02870D8}">
   <dimension ref="A2:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
@@ -6555,7 +6555,7 @@
   <sheetPr codeName="Planilha7"/>
   <dimension ref="A2:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -6952,9 +6952,9 @@
   <sheetPr codeName="Planilha8"/>
   <dimension ref="A2:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7:G7"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7497,17 +7497,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6f36a527-e39f-47ee-9db9-a20740d34e39" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fcbf2d89-ce9d-4bbe-8922-6cf9cd327567">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005542DEAA73BD554594037CA22C04B274" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="b5107fdb2837f701ae9b29e980f5730d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fcbf2d89-ce9d-4bbe-8922-6cf9cd327567" xmlns:ns3="6f36a527-e39f-47ee-9db9-a20740d34e39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="18585c6c93e8f3576b52f07c08d00791" ns2:_="" ns3:_="">
     <xsd:import namespace="fcbf2d89-ce9d-4bbe-8922-6cf9cd327567"/>
@@ -7736,6 +7725,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6f36a527-e39f-47ee-9db9-a20740d34e39" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fcbf2d89-ce9d-4bbe-8922-6cf9cd327567">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7746,17 +7746,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AA22D7F-B900-4856-B4A0-B450CEAE443D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6f36a527-e39f-47ee-9db9-a20740d34e39"/>
-    <ds:schemaRef ds:uri="fcbf2d89-ce9d-4bbe-8922-6cf9cd327567"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F897654-2AD2-49BB-9B02-99C6AD8B26B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7775,6 +7764,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AA22D7F-B900-4856-B4A0-B450CEAE443D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6f36a527-e39f-47ee-9db9-a20740d34e39"/>
+    <ds:schemaRef ds:uri="fcbf2d89-ce9d-4bbe-8922-6cf9cd327567"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D3FBA05-872E-4201-A0CD-8310D7A6AB5A}">
   <ds:schemaRefs>

</xml_diff>